<commit_message>
Share Invoice Remaining testcases and keywords
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/share_invoice_test_data.xlsx
+++ b/TestData/Web_POS/Billing/share_invoice_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="227" count="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="232" count="202">
   <si>
     <t>TC_Id</t>
   </si>
@@ -695,6 +695,21 @@
   </si>
   <si>
     <t>SI_10</t>
+  </si>
+  <si>
+    <t>SI_11</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>abc@gmail.com</t>
+  </si>
+  <si>
+    <t>SI_12</t>
   </si>
 </sst>
 </file>
@@ -1053,7 +1068,7 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView topLeftCell="L45" view="normal" tabSelected="1" workbookViewId="0">
       <selection pane="topLeft" activeCell="R66" sqref="R66"/>
@@ -1078,7 +1093,7 @@
     <col min="20" max="20" width="12.84765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" customHeight="1">
+    <row r="1" spans="1:21" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1139,8 +1154,11 @@
       <c r="T1" t="s">
         <v>213</v>
       </c>
+      <c r="U1" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="2" spans="1:20" ht="33.75" customHeight="1">
+    <row r="2" spans="1:21" ht="33.75" customHeight="1">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1201,8 +1219,11 @@
       <c r="T2">
         <v>7709577438</v>
       </c>
+      <c r="U2" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -1263,8 +1284,11 @@
       <c r="T3">
         <v>7709577438</v>
       </c>
+      <c r="U3" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -1325,8 +1349,11 @@
       <c r="T4">
         <v>7709577438</v>
       </c>
+      <c r="U4" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>220</v>
       </c>
@@ -1387,8 +1414,11 @@
       <c r="T5">
         <v>7709577438</v>
       </c>
+      <c r="U5" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -1449,8 +1479,11 @@
       <c r="T6">
         <v>7709577438</v>
       </c>
+      <c r="U6" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -1511,8 +1544,11 @@
       <c r="T7">
         <v>7709577438</v>
       </c>
+      <c r="U7" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>223</v>
       </c>
@@ -1573,8 +1609,11 @@
       <c r="T8">
         <v>7709577438</v>
       </c>
+      <c r="U8" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -1635,8 +1674,11 @@
       <c r="T9">
         <v>7709577438</v>
       </c>
+      <c r="U9" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>225</v>
       </c>
@@ -1697,8 +1739,11 @@
       <c r="T10">
         <v>7709577438</v>
       </c>
+      <c r="U10" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>226</v>
       </c>
@@ -1759,8 +1804,140 @@
       <c r="T11">
         <v>7709577438</v>
       </c>
+      <c r="U11" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="13" ht="15"/>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>227</v>
+      </c>
+      <c r="B12" t="s">
+        <v>200</v>
+      </c>
+      <c r="C12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12">
+        <v>123456</v>
+      </c>
+      <c r="E12" t="s">
+        <v>199</v>
+      </c>
+      <c r="F12">
+        <v>123456</v>
+      </c>
+      <c r="G12">
+        <v>1000</v>
+      </c>
+      <c r="H12">
+        <v>600</v>
+      </c>
+      <c r="I12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" t="s">
+        <v>25</v>
+      </c>
+      <c r="O12" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P12" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S12" t="s">
+        <v>211</v>
+      </c>
+      <c r="T12">
+        <v>7709577438</v>
+      </c>
+      <c r="U12" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>231</v>
+      </c>
+      <c r="B13" t="s">
+        <v>200</v>
+      </c>
+      <c r="C13" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13">
+        <v>123456</v>
+      </c>
+      <c r="E13" t="s">
+        <v>199</v>
+      </c>
+      <c r="F13">
+        <v>123456</v>
+      </c>
+      <c r="G13">
+        <v>1000</v>
+      </c>
+      <c r="H13">
+        <v>600</v>
+      </c>
+      <c r="I13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M13" t="s">
+        <v>24</v>
+      </c>
+      <c r="N13" t="s">
+        <v>25</v>
+      </c>
+      <c r="O13" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>27</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S13" t="s">
+        <v>211</v>
+      </c>
+      <c r="T13">
+        <v>7709577438</v>
+      </c>
+      <c r="U13" t="s">
+        <v>229</v>
+      </c>
+    </row>
     <row r="15" ht="15"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Share Invoice All testcases and keywords
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/share_invoice_test_data.xlsx
+++ b/TestData/Web_POS/Billing/share_invoice_test_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="232" count="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="246" count="414">
   <si>
     <t>TC_Id</t>
   </si>
@@ -700,7 +700,7 @@
     <t>SI_11</t>
   </si>
   <si>
-    <t>email</t>
+    <t>cust_email</t>
   </si>
   <si>
     <t>Null</t>
@@ -710,6 +710,48 @@
   </si>
   <si>
     <t>SI_12</t>
+  </si>
+  <si>
+    <t>SI_13</t>
+  </si>
+  <si>
+    <t>SI_14</t>
+  </si>
+  <si>
+    <t>SI_15</t>
+  </si>
+  <si>
+    <t>SI_16</t>
+  </si>
+  <si>
+    <t>SI_17</t>
+  </si>
+  <si>
+    <t>abc@gm</t>
+  </si>
+  <si>
+    <t>SI_18</t>
+  </si>
+  <si>
+    <t>SI_19</t>
+  </si>
+  <si>
+    <t>SI_20</t>
+  </si>
+  <si>
+    <t>dprimaryuser@gmail.com</t>
+  </si>
+  <si>
+    <t>dprimaryuser2@gmail.com</t>
+  </si>
+  <si>
+    <t>SI_21</t>
+  </si>
+  <si>
+    <t>SI_22</t>
+  </si>
+  <si>
+    <t>update_email</t>
   </si>
 </sst>
 </file>
@@ -790,7 +832,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -812,11 +861,11 @@
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="0" applyBorder="0" applyNumberFormat="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyFont="1" applyFill="1"/>
@@ -1068,7 +1117,7 @@
   <sheetPr>
     <outlinePr summaryRight="0" summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView topLeftCell="L45" view="normal" tabSelected="1" workbookViewId="0">
       <selection pane="topLeft" activeCell="R66" sqref="R66"/>
@@ -1093,7 +1142,7 @@
     <col min="20" max="20" width="12.84765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" customHeight="1">
+    <row r="1" spans="1:22" customHeight="1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1157,8 +1206,11 @@
       <c r="U1" t="s">
         <v>228</v>
       </c>
+      <c r="V1" t="s">
+        <v>245</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" ht="33.75" customHeight="1">
+    <row r="2" spans="1:22" ht="33.75" customHeight="1">
       <c r="A2" t="s">
         <v>107</v>
       </c>
@@ -1222,8 +1274,11 @@
       <c r="U2" t="s">
         <v>229</v>
       </c>
+      <c r="V2" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>207</v>
       </c>
@@ -1287,8 +1342,11 @@
       <c r="U3" t="s">
         <v>229</v>
       </c>
+      <c r="V3" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>219</v>
       </c>
@@ -1352,8 +1410,11 @@
       <c r="U4" t="s">
         <v>229</v>
       </c>
+      <c r="V4" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>220</v>
       </c>
@@ -1417,8 +1478,11 @@
       <c r="U5" t="s">
         <v>229</v>
       </c>
+      <c r="V5" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>221</v>
       </c>
@@ -1482,8 +1546,11 @@
       <c r="U6" t="s">
         <v>229</v>
       </c>
+      <c r="V6" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>222</v>
       </c>
@@ -1547,8 +1614,11 @@
       <c r="U7" t="s">
         <v>229</v>
       </c>
+      <c r="V7" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>223</v>
       </c>
@@ -1612,8 +1682,11 @@
       <c r="U8" t="s">
         <v>229</v>
       </c>
+      <c r="V8" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>224</v>
       </c>
@@ -1677,8 +1750,11 @@
       <c r="U9" t="s">
         <v>229</v>
       </c>
+      <c r="V9" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="10" spans="1:21">
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>225</v>
       </c>
@@ -1742,8 +1818,11 @@
       <c r="U10" t="s">
         <v>229</v>
       </c>
+      <c r="V10" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="11" spans="1:21">
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>226</v>
       </c>
@@ -1807,8 +1886,11 @@
       <c r="U11" t="s">
         <v>229</v>
       </c>
+      <c r="V11" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="12" spans="1:21">
+    <row r="12" spans="1:22">
       <c r="A12" t="s">
         <v>227</v>
       </c>
@@ -1872,8 +1954,11 @@
       <c r="U12" t="s">
         <v>230</v>
       </c>
+      <c r="V12" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="13" spans="1:21">
+    <row r="13" spans="1:22">
       <c r="A13" t="s">
         <v>231</v>
       </c>
@@ -1937,8 +2022,691 @@
       <c r="U13" t="s">
         <v>229</v>
       </c>
+      <c r="V13" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="15" ht="15"/>
+    <row r="14" spans="1:22">
+      <c r="A14" t="s">
+        <v>232</v>
+      </c>
+      <c r="B14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>123456</v>
+      </c>
+      <c r="E14" t="s">
+        <v>199</v>
+      </c>
+      <c r="F14">
+        <v>123456</v>
+      </c>
+      <c r="G14">
+        <v>1000</v>
+      </c>
+      <c r="H14">
+        <v>600</v>
+      </c>
+      <c r="I14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M14" t="s">
+        <v>24</v>
+      </c>
+      <c r="N14" t="s">
+        <v>25</v>
+      </c>
+      <c r="O14" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P14" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>27</v>
+      </c>
+      <c r="R14" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S14" t="s">
+        <v>211</v>
+      </c>
+      <c r="T14">
+        <v>7709577438</v>
+      </c>
+      <c r="U14" t="s">
+        <v>229</v>
+      </c>
+      <c r="V14" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
+      <c r="A15" t="s">
+        <v>233</v>
+      </c>
+      <c r="B15" t="s">
+        <v>200</v>
+      </c>
+      <c r="C15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15">
+        <v>123456</v>
+      </c>
+      <c r="E15" t="s">
+        <v>199</v>
+      </c>
+      <c r="F15">
+        <v>123456</v>
+      </c>
+      <c r="G15">
+        <v>1000</v>
+      </c>
+      <c r="H15">
+        <v>600</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" t="s">
+        <v>24</v>
+      </c>
+      <c r="N15" t="s">
+        <v>25</v>
+      </c>
+      <c r="O15" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P15" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S15" t="s">
+        <v>211</v>
+      </c>
+      <c r="T15">
+        <v>7709577438</v>
+      </c>
+      <c r="U15" t="s">
+        <v>229</v>
+      </c>
+      <c r="V15" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" t="s">
+        <v>234</v>
+      </c>
+      <c r="B16" t="s">
+        <v>200</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16">
+        <v>123456</v>
+      </c>
+      <c r="E16" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16">
+        <v>123456</v>
+      </c>
+      <c r="G16">
+        <v>1000</v>
+      </c>
+      <c r="H16">
+        <v>600</v>
+      </c>
+      <c r="I16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" t="s">
+        <v>24</v>
+      </c>
+      <c r="N16" t="s">
+        <v>25</v>
+      </c>
+      <c r="O16" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P16" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>27</v>
+      </c>
+      <c r="R16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S16" t="s">
+        <v>211</v>
+      </c>
+      <c r="T16">
+        <v>77095774</v>
+      </c>
+      <c r="U16" t="s">
+        <v>229</v>
+      </c>
+      <c r="V16" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
+      <c r="A17" t="s">
+        <v>235</v>
+      </c>
+      <c r="B17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17">
+        <v>123456</v>
+      </c>
+      <c r="E17" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17">
+        <v>123456</v>
+      </c>
+      <c r="G17">
+        <v>1000</v>
+      </c>
+      <c r="H17">
+        <v>600</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P17" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>27</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S17" t="s">
+        <v>211</v>
+      </c>
+      <c r="T17">
+        <v>7709577438</v>
+      </c>
+      <c r="U17" t="s">
+        <v>230</v>
+      </c>
+      <c r="V17" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
+      <c r="A18" t="s">
+        <v>236</v>
+      </c>
+      <c r="B18" t="s">
+        <v>200</v>
+      </c>
+      <c r="C18" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18">
+        <v>123456</v>
+      </c>
+      <c r="E18" t="s">
+        <v>199</v>
+      </c>
+      <c r="F18">
+        <v>123456</v>
+      </c>
+      <c r="G18">
+        <v>1000</v>
+      </c>
+      <c r="H18">
+        <v>600</v>
+      </c>
+      <c r="I18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L18" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M18" t="s">
+        <v>24</v>
+      </c>
+      <c r="N18" t="s">
+        <v>25</v>
+      </c>
+      <c r="O18" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P18" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>27</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S18" t="s">
+        <v>211</v>
+      </c>
+      <c r="T18">
+        <v>7709577438</v>
+      </c>
+      <c r="U18" t="s">
+        <v>237</v>
+      </c>
+      <c r="V18" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
+      <c r="A19" t="s">
+        <v>238</v>
+      </c>
+      <c r="B19" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19">
+        <v>123456</v>
+      </c>
+      <c r="E19" t="s">
+        <v>199</v>
+      </c>
+      <c r="F19">
+        <v>123456</v>
+      </c>
+      <c r="G19">
+        <v>1000</v>
+      </c>
+      <c r="H19">
+        <v>600</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M19" t="s">
+        <v>24</v>
+      </c>
+      <c r="N19" t="s">
+        <v>25</v>
+      </c>
+      <c r="O19" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P19" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>27</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S19" t="s">
+        <v>211</v>
+      </c>
+      <c r="T19">
+        <v>7709577438</v>
+      </c>
+      <c r="U19" t="s">
+        <v>237</v>
+      </c>
+      <c r="V19" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
+      <c r="A20" t="s">
+        <v>239</v>
+      </c>
+      <c r="B20" t="s">
+        <v>200</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <v>123456</v>
+      </c>
+      <c r="E20" t="s">
+        <v>199</v>
+      </c>
+      <c r="F20">
+        <v>123456</v>
+      </c>
+      <c r="G20">
+        <v>1000</v>
+      </c>
+      <c r="H20">
+        <v>600</v>
+      </c>
+      <c r="I20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" t="s">
+        <v>24</v>
+      </c>
+      <c r="N20" t="s">
+        <v>25</v>
+      </c>
+      <c r="O20" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P20" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>27</v>
+      </c>
+      <c r="R20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S20" t="s">
+        <v>211</v>
+      </c>
+      <c r="T20">
+        <v>7709577438</v>
+      </c>
+      <c r="U20" t="s">
+        <v>241</v>
+      </c>
+      <c r="V20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
+      <c r="A21" t="s">
+        <v>240</v>
+      </c>
+      <c r="B21" t="s">
+        <v>200</v>
+      </c>
+      <c r="C21" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <v>123456</v>
+      </c>
+      <c r="E21" t="s">
+        <v>199</v>
+      </c>
+      <c r="F21">
+        <v>123456</v>
+      </c>
+      <c r="G21">
+        <v>1000</v>
+      </c>
+      <c r="H21">
+        <v>600</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L21" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M21" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" t="s">
+        <v>25</v>
+      </c>
+      <c r="O21" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P21" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>27</v>
+      </c>
+      <c r="R21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S21" t="s">
+        <v>211</v>
+      </c>
+      <c r="T21">
+        <v>7709577438</v>
+      </c>
+      <c r="U21" t="s">
+        <v>241</v>
+      </c>
+      <c r="V21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23">
+      <c r="A22" t="s">
+        <v>243</v>
+      </c>
+      <c r="B22" t="s">
+        <v>200</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>123456</v>
+      </c>
+      <c r="E22" t="s">
+        <v>199</v>
+      </c>
+      <c r="F22">
+        <v>123456</v>
+      </c>
+      <c r="G22">
+        <v>1000</v>
+      </c>
+      <c r="H22">
+        <v>600</v>
+      </c>
+      <c r="I22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L22" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M22" t="s">
+        <v>24</v>
+      </c>
+      <c r="N22" t="s">
+        <v>25</v>
+      </c>
+      <c r="O22" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P22" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>27</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S22" t="s">
+        <v>211</v>
+      </c>
+      <c r="T22">
+        <v>7709577438</v>
+      </c>
+      <c r="U22" t="s">
+        <v>241</v>
+      </c>
+      <c r="V22" t="s">
+        <v>242</v>
+      </c>
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="1:22">
+      <c r="A23" t="s">
+        <v>244</v>
+      </c>
+      <c r="B23" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <v>123456</v>
+      </c>
+      <c r="E23" t="s">
+        <v>199</v>
+      </c>
+      <c r="F23">
+        <v>123456</v>
+      </c>
+      <c r="G23">
+        <v>1000</v>
+      </c>
+      <c r="H23">
+        <v>600</v>
+      </c>
+      <c r="I23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="K23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>25</v>
+      </c>
+      <c r="O23" s="15">
+        <v>45384</v>
+      </c>
+      <c r="P23" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>27</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S23" t="s">
+        <v>211</v>
+      </c>
+      <c r="T23">
+        <v>7709577438</v>
+      </c>
+      <c r="U23" t="s">
+        <v>229</v>
+      </c>
+      <c r="V23" s="6" t="s">
+        <v>229</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter scaleWithDoc="1" alignWithMargins="0" differentFirst="0" differentOddEven="0"/>

</xml_diff>

<commit_message>
Assertion keyword of share invoice updated
</commit_message>
<xml_diff>
--- a/TestData/Web_POS/Billing/share_invoice_test_data.xlsx
+++ b/TestData/Web_POS/Billing/share_invoice_test_data.xlsx
@@ -2625,10 +2625,10 @@
         <v>7709577438</v>
       </c>
       <c r="U22" t="s">
+        <v>242</v>
+      </c>
+      <c r="V22" t="s">
         <v>241</v>
-      </c>
-      <c r="V22" t="s">
-        <v>242</v>
       </c>
       <c r="W22" s="6"/>
     </row>

</xml_diff>